<commit_message>
a Adjusting the test cases to fit the new logic
</commit_message>
<xml_diff>
--- a/src/test/resources/test_files/original/Test_Input.xlsx
+++ b/src/test/resources/test_files/original/Test_Input.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\malhaq\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://airarabia-my.sharepoint.com/personal/malhaq_isa_ae1/Documents/Documents/ExcelColumnConvert/ExcelColumnConvert/src/test/resources/test_files/original/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{309DD13E-0650-465F-8F65-73653ABF23D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>

</xml_diff>

<commit_message>
converting between excel files with out the need of creating a new file
</commit_message>
<xml_diff>
--- a/src/test/resources/test_files/original/Test_Input.xlsx
+++ b/src/test/resources/test_files/original/Test_Input.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://airarabia-my.sharepoint.com/personal/malhaq_isa_ae1/Documents/Documents/ExcelColumnConvert/ExcelColumnConvert/src/test/resources/test_files/original/"/>
     </mc:Choice>
@@ -179,6 +179,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -520,7 +521,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F18" sqref="F18"/>
@@ -528,291 +529,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="18.28515625" customWidth="1"/>
-    <col min="4" max="4" width="48.7109375" customWidth="1"/>
+    <col min="3" max="3" customWidth="true" width="18.28515625"/>
+    <col min="4" max="4" customWidth="true" width="48.7109375"/>
   </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1">
-        <v>25</v>
-      </c>
-      <c r="C1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>30</v>
-      </c>
-      <c r="C2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3">
-        <v>22</v>
-      </c>
-      <c r="C3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4">
-        <v>28</v>
-      </c>
-      <c r="C4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5">
-        <v>35</v>
-      </c>
-      <c r="C5" t="s">
-        <v>24</v>
-      </c>
-      <c r="D5" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6">
-        <v>40</v>
-      </c>
-      <c r="C6" t="s">
-        <v>25</v>
-      </c>
-      <c r="D6" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7">
-        <v>19</v>
-      </c>
-      <c r="C7" t="s">
-        <v>26</v>
-      </c>
-      <c r="D7" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8">
-        <v>21</v>
-      </c>
-      <c r="C8" t="s">
-        <v>27</v>
-      </c>
-      <c r="D8" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9">
-        <v>45</v>
-      </c>
-      <c r="C9" t="s">
-        <v>28</v>
-      </c>
-      <c r="D9" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10">
-        <v>50</v>
-      </c>
-      <c r="C10" t="s">
-        <v>29</v>
-      </c>
-      <c r="D10" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11">
-        <v>33</v>
-      </c>
-      <c r="C11" t="s">
-        <v>30</v>
-      </c>
-      <c r="D11" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>11</v>
-      </c>
-      <c r="B12">
-        <v>27</v>
-      </c>
-      <c r="C12" t="s">
-        <v>31</v>
-      </c>
-      <c r="D12" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>12</v>
-      </c>
-      <c r="B13">
-        <v>31</v>
-      </c>
-      <c r="C13" t="s">
-        <v>32</v>
-      </c>
-      <c r="D13" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14">
-        <v>29</v>
-      </c>
-      <c r="C14" t="s">
-        <v>33</v>
-      </c>
-      <c r="D14" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>14</v>
-      </c>
-      <c r="B15">
-        <v>26</v>
-      </c>
-      <c r="C15" t="s">
-        <v>34</v>
-      </c>
-      <c r="D15" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>15</v>
-      </c>
-      <c r="B16">
-        <v>38</v>
-      </c>
-      <c r="C16" t="s">
-        <v>35</v>
-      </c>
-      <c r="D16" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>16</v>
-      </c>
-      <c r="B17">
-        <v>41</v>
-      </c>
-      <c r="C17" t="s">
-        <v>36</v>
-      </c>
-      <c r="D17" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>17</v>
-      </c>
-      <c r="B18">
-        <v>20</v>
-      </c>
-      <c r="C18" t="s">
-        <v>37</v>
-      </c>
-      <c r="D18" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>18</v>
-      </c>
-      <c r="B19">
-        <v>32</v>
-      </c>
-      <c r="C19" t="s">
-        <v>38</v>
-      </c>
-      <c r="D19" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>19</v>
-      </c>
-      <c r="B20">
-        <v>37</v>
-      </c>
-      <c r="C20" t="s">
-        <v>39</v>
-      </c>
-      <c r="D20" t="s">
-        <v>46</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter>

</xml_diff>

<commit_message>
fixing the testing issue for ConvertExcelTest
</commit_message>
<xml_diff>
--- a/src/test/resources/test_files/original/Test_Input.xlsx
+++ b/src/test/resources/test_files/original/Test_Input.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://airarabia-my.sharepoint.com/personal/malhaq_isa_ae1/Documents/Documents/ExcelColumnConvert/ExcelColumnConvert/src/test/resources/test_files/original/"/>
     </mc:Choice>
@@ -179,7 +179,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -521,7 +520,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F18" sqref="F18"/>
@@ -529,10 +528,291 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" customWidth="true" width="18.28515625"/>
-    <col min="4" max="4" customWidth="true" width="48.7109375"/>
+    <col min="3" max="3" width="18.28515625" customWidth="1"/>
+    <col min="4" max="4" width="48.7109375" customWidth="1"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1">
+        <v>25</v>
+      </c>
+      <c r="C1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>30</v>
+      </c>
+      <c r="C2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>22</v>
+      </c>
+      <c r="C3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>28</v>
+      </c>
+      <c r="C4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>35</v>
+      </c>
+      <c r="C5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>40</v>
+      </c>
+      <c r="C6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>19</v>
+      </c>
+      <c r="C7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>21</v>
+      </c>
+      <c r="C8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>45</v>
+      </c>
+      <c r="C9" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>50</v>
+      </c>
+      <c r="C10" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>33</v>
+      </c>
+      <c r="C11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>27</v>
+      </c>
+      <c r="C12" t="s">
+        <v>31</v>
+      </c>
+      <c r="D12" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>31</v>
+      </c>
+      <c r="C13" t="s">
+        <v>32</v>
+      </c>
+      <c r="D13" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>29</v>
+      </c>
+      <c r="C14" t="s">
+        <v>33</v>
+      </c>
+      <c r="D14" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>26</v>
+      </c>
+      <c r="C15" t="s">
+        <v>34</v>
+      </c>
+      <c r="D15" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>38</v>
+      </c>
+      <c r="C16" t="s">
+        <v>35</v>
+      </c>
+      <c r="D16" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <v>41</v>
+      </c>
+      <c r="C17" t="s">
+        <v>36</v>
+      </c>
+      <c r="D17" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <v>20</v>
+      </c>
+      <c r="C18" t="s">
+        <v>37</v>
+      </c>
+      <c r="D18" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19">
+        <v>32</v>
+      </c>
+      <c r="C19" t="s">
+        <v>38</v>
+      </c>
+      <c r="D19" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20">
+        <v>37</v>
+      </c>
+      <c r="C20" t="s">
+        <v>39</v>
+      </c>
+      <c r="D20" t="s">
+        <v>46</v>
+      </c>
+    </row>
+  </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter>

</xml_diff>

<commit_message>
adding SheetOrientation to change Excel sheet orientation and page size
</commit_message>
<xml_diff>
--- a/src/test/resources/test_files/original/Test_Input.xlsx
+++ b/src/test/resources/test_files/original/Test_Input.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://airarabia-my.sharepoint.com/personal/malhaq_isa_ae1/Documents/Documents/ExcelColumnConvert/ExcelColumnConvert/src/test/resources/test_files/original/"/>
     </mc:Choice>
@@ -179,6 +179,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -520,7 +521,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F18" sqref="F18"/>
@@ -528,291 +529,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="18.28515625" customWidth="1"/>
-    <col min="4" max="4" width="48.7109375" customWidth="1"/>
+    <col min="3" max="3" customWidth="true" width="18.28515625"/>
+    <col min="4" max="4" customWidth="true" width="48.7109375"/>
   </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1">
-        <v>25</v>
-      </c>
-      <c r="C1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>30</v>
-      </c>
-      <c r="C2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3">
-        <v>22</v>
-      </c>
-      <c r="C3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4">
-        <v>28</v>
-      </c>
-      <c r="C4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5">
-        <v>35</v>
-      </c>
-      <c r="C5" t="s">
-        <v>24</v>
-      </c>
-      <c r="D5" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6">
-        <v>40</v>
-      </c>
-      <c r="C6" t="s">
-        <v>25</v>
-      </c>
-      <c r="D6" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7">
-        <v>19</v>
-      </c>
-      <c r="C7" t="s">
-        <v>26</v>
-      </c>
-      <c r="D7" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8">
-        <v>21</v>
-      </c>
-      <c r="C8" t="s">
-        <v>27</v>
-      </c>
-      <c r="D8" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9">
-        <v>45</v>
-      </c>
-      <c r="C9" t="s">
-        <v>28</v>
-      </c>
-      <c r="D9" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10">
-        <v>50</v>
-      </c>
-      <c r="C10" t="s">
-        <v>29</v>
-      </c>
-      <c r="D10" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11">
-        <v>33</v>
-      </c>
-      <c r="C11" t="s">
-        <v>30</v>
-      </c>
-      <c r="D11" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>11</v>
-      </c>
-      <c r="B12">
-        <v>27</v>
-      </c>
-      <c r="C12" t="s">
-        <v>31</v>
-      </c>
-      <c r="D12" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>12</v>
-      </c>
-      <c r="B13">
-        <v>31</v>
-      </c>
-      <c r="C13" t="s">
-        <v>32</v>
-      </c>
-      <c r="D13" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14">
-        <v>29</v>
-      </c>
-      <c r="C14" t="s">
-        <v>33</v>
-      </c>
-      <c r="D14" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>14</v>
-      </c>
-      <c r="B15">
-        <v>26</v>
-      </c>
-      <c r="C15" t="s">
-        <v>34</v>
-      </c>
-      <c r="D15" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>15</v>
-      </c>
-      <c r="B16">
-        <v>38</v>
-      </c>
-      <c r="C16" t="s">
-        <v>35</v>
-      </c>
-      <c r="D16" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>16</v>
-      </c>
-      <c r="B17">
-        <v>41</v>
-      </c>
-      <c r="C17" t="s">
-        <v>36</v>
-      </c>
-      <c r="D17" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>17</v>
-      </c>
-      <c r="B18">
-        <v>20</v>
-      </c>
-      <c r="C18" t="s">
-        <v>37</v>
-      </c>
-      <c r="D18" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>18</v>
-      </c>
-      <c r="B19">
-        <v>32</v>
-      </c>
-      <c r="C19" t="s">
-        <v>38</v>
-      </c>
-      <c r="D19" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>19</v>
-      </c>
-      <c r="B20">
-        <v>37</v>
-      </c>
-      <c r="C20" t="s">
-        <v>39</v>
-      </c>
-      <c r="D20" t="s">
-        <v>46</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter>

</xml_diff>

<commit_message>
optimizing the delete logic and adding support of two condition to delete by condition action
</commit_message>
<xml_diff>
--- a/src/test/resources/test_files/original/Test_Input.xlsx
+++ b/src/test/resources/test_files/original/Test_Input.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://airarabia-my.sharepoint.com/personal/malhaq_isa_ae1/Documents/Documents/ExcelColumnConvert/ExcelColumnConvert/src/test/resources/test_files/original/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\malhaq\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{309DD13E-0650-465F-8F65-73653ABF23D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -179,7 +179,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -521,7 +520,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F18" sqref="F18"/>
@@ -529,10 +528,291 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" customWidth="true" width="18.28515625"/>
-    <col min="4" max="4" customWidth="true" width="48.7109375"/>
+    <col min="3" max="3" width="18.28515625" customWidth="1"/>
+    <col min="4" max="4" width="48.7109375" customWidth="1"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1">
+        <v>25</v>
+      </c>
+      <c r="C1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>30</v>
+      </c>
+      <c r="C2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>22</v>
+      </c>
+      <c r="C3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>28</v>
+      </c>
+      <c r="C4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>35</v>
+      </c>
+      <c r="C5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>40</v>
+      </c>
+      <c r="C6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>19</v>
+      </c>
+      <c r="C7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>21</v>
+      </c>
+      <c r="C8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>45</v>
+      </c>
+      <c r="C9" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>50</v>
+      </c>
+      <c r="C10" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>33</v>
+      </c>
+      <c r="C11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>27</v>
+      </c>
+      <c r="C12" t="s">
+        <v>31</v>
+      </c>
+      <c r="D12" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>31</v>
+      </c>
+      <c r="C13" t="s">
+        <v>32</v>
+      </c>
+      <c r="D13" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>29</v>
+      </c>
+      <c r="C14" t="s">
+        <v>33</v>
+      </c>
+      <c r="D14" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>26</v>
+      </c>
+      <c r="C15" t="s">
+        <v>34</v>
+      </c>
+      <c r="D15" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>38</v>
+      </c>
+      <c r="C16" t="s">
+        <v>35</v>
+      </c>
+      <c r="D16" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <v>41</v>
+      </c>
+      <c r="C17" t="s">
+        <v>36</v>
+      </c>
+      <c r="D17" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <v>20</v>
+      </c>
+      <c r="C18" t="s">
+        <v>37</v>
+      </c>
+      <c r="D18" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19">
+        <v>32</v>
+      </c>
+      <c r="C19" t="s">
+        <v>38</v>
+      </c>
+      <c r="D19" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20">
+        <v>37</v>
+      </c>
+      <c r="C20" t="s">
+        <v>39</v>
+      </c>
+      <c r="D20" t="s">
+        <v>46</v>
+      </c>
+    </row>
+  </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter>

</xml_diff>

<commit_message>
Adding new action to sort excel sheets
</commit_message>
<xml_diff>
--- a/src/test/resources/test_files/original/Test_Input.xlsx
+++ b/src/test/resources/test_files/original/Test_Input.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\malhaq\Downloads\"/>
     </mc:Choice>
@@ -179,6 +179,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -520,7 +521,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F18" sqref="F18"/>
@@ -528,291 +529,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="18.28515625" customWidth="1"/>
-    <col min="4" max="4" width="48.7109375" customWidth="1"/>
+    <col min="3" max="3" customWidth="true" width="18.28515625"/>
+    <col min="4" max="4" customWidth="true" width="48.7109375"/>
   </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1">
-        <v>25</v>
-      </c>
-      <c r="C1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>30</v>
-      </c>
-      <c r="C2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3">
-        <v>22</v>
-      </c>
-      <c r="C3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4">
-        <v>28</v>
-      </c>
-      <c r="C4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5">
-        <v>35</v>
-      </c>
-      <c r="C5" t="s">
-        <v>24</v>
-      </c>
-      <c r="D5" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6">
-        <v>40</v>
-      </c>
-      <c r="C6" t="s">
-        <v>25</v>
-      </c>
-      <c r="D6" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7">
-        <v>19</v>
-      </c>
-      <c r="C7" t="s">
-        <v>26</v>
-      </c>
-      <c r="D7" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8">
-        <v>21</v>
-      </c>
-      <c r="C8" t="s">
-        <v>27</v>
-      </c>
-      <c r="D8" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9">
-        <v>45</v>
-      </c>
-      <c r="C9" t="s">
-        <v>28</v>
-      </c>
-      <c r="D9" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10">
-        <v>50</v>
-      </c>
-      <c r="C10" t="s">
-        <v>29</v>
-      </c>
-      <c r="D10" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11">
-        <v>33</v>
-      </c>
-      <c r="C11" t="s">
-        <v>30</v>
-      </c>
-      <c r="D11" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>11</v>
-      </c>
-      <c r="B12">
-        <v>27</v>
-      </c>
-      <c r="C12" t="s">
-        <v>31</v>
-      </c>
-      <c r="D12" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>12</v>
-      </c>
-      <c r="B13">
-        <v>31</v>
-      </c>
-      <c r="C13" t="s">
-        <v>32</v>
-      </c>
-      <c r="D13" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14">
-        <v>29</v>
-      </c>
-      <c r="C14" t="s">
-        <v>33</v>
-      </c>
-      <c r="D14" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>14</v>
-      </c>
-      <c r="B15">
-        <v>26</v>
-      </c>
-      <c r="C15" t="s">
-        <v>34</v>
-      </c>
-      <c r="D15" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>15</v>
-      </c>
-      <c r="B16">
-        <v>38</v>
-      </c>
-      <c r="C16" t="s">
-        <v>35</v>
-      </c>
-      <c r="D16" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>16</v>
-      </c>
-      <c r="B17">
-        <v>41</v>
-      </c>
-      <c r="C17" t="s">
-        <v>36</v>
-      </c>
-      <c r="D17" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>17</v>
-      </c>
-      <c r="B18">
-        <v>20</v>
-      </c>
-      <c r="C18" t="s">
-        <v>37</v>
-      </c>
-      <c r="D18" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>18</v>
-      </c>
-      <c r="B19">
-        <v>32</v>
-      </c>
-      <c r="C19" t="s">
-        <v>38</v>
-      </c>
-      <c r="D19" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>19</v>
-      </c>
-      <c r="B20">
-        <v>37</v>
-      </c>
-      <c r="C20" t="s">
-        <v>39</v>
-      </c>
-      <c r="D20" t="s">
-        <v>46</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter>

</xml_diff>